<commit_message>
Sum of even & odd
</commit_message>
<xml_diff>
--- a/Resources/Index.xlsx
+++ b/Resources/Index.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="53">
   <si>
     <t>Sr No.</t>
   </si>
@@ -160,13 +160,34 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Sum of even &amp; odd</t>
+  </si>
+  <si>
+    <t>Sliding Window</t>
+  </si>
+  <si>
+    <t>Max &amp; Min Sum</t>
+  </si>
+  <si>
+    <t>Array Manipulation</t>
+  </si>
+  <si>
+    <t>Prefix Sum</t>
+  </si>
+  <si>
+    <t>Sum of Elements</t>
+  </si>
+  <si>
+    <t>Even-Odd Calculation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +225,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -526,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -642,12 +671,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="98">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1597,8 +1671,8 @@
   <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2032,7 +2106,7 @@
       <c r="S8" s="8"/>
       <c r="T8"/>
     </row>
-    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>6</v>
       </c>
@@ -2042,21 +2116,29 @@
       <c r="C9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17" t="s">
+      <c r="D9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="F9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="I9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K9" s="37" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>45</v>
@@ -2073,10 +2155,10 @@
       <c r="P9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9" s="20" t="s">
+      <c r="Q9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="S9" s="8"/>
@@ -2084,41 +2166,53 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>50</v>
+      </c>
       <c r="E10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="19" t="s">
+      <c r="F10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="21" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K10" s="38" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="M10" s="38" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="N10" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="21" t="s">
         <v>20</v>
       </c>
       <c r="Q10" s="20" t="s">
@@ -3274,9 +3368,14 @@
       <c r="R37" s="3"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -3289,12 +3388,10 @@
       <c r="R38" s="3"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
+      <c r="A39"/>
       <c r="B39"/>
-      <c r="D39"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="C39"/>
+      <c r="E39"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -3307,9 +3404,10 @@
       <c r="R39" s="3"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
-      <c r="D40"/>
+      <c r="E40"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B41"/>
@@ -3349,333 +3447,344 @@
     <mergeCell ref="E1:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J7">
-    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="97" priority="95" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="93" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="96" priority="96" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="94" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="95" priority="97" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="95" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K7">
-    <cfRule type="containsText" dxfId="87" priority="88" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="93" priority="91" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="89" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="92" priority="92" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="90" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="91" priority="93" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="91" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N7">
-    <cfRule type="containsText" dxfId="83" priority="84" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="89" priority="87" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="85" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="88" priority="88" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="86" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="87" priority="89" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="87" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="86" priority="90" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",M4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:T7">
-    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="85" priority="83" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="84" priority="84" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="82" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="83" priority="85" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="83" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",T4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 E6:E7 E32:E33">
-    <cfRule type="containsText" dxfId="75" priority="77" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="81" priority="80" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="78" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="79" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="79" priority="82" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T9:T11">
-    <cfRule type="containsText" dxfId="72" priority="74" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="78" priority="77" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",T9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="75" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",T9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="76" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="76" priority="79" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",T9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32:N35 J32:K35">
-    <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="75" priority="73" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="71" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="74" priority="74" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="72" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="73" priority="75" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="73" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="72" priority="76" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E35">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="71" priority="67" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="68" priority="64" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E9">
-    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="Hard">
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="65" priority="61" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="64" priority="62" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:N11 J8:K11">
-    <cfRule type="containsText" dxfId="56" priority="54" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="62" priority="57" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="55" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="61" priority="58" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="56" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="60" priority="59" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="57" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E11">
-    <cfRule type="containsText" dxfId="52" priority="51" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="53" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E10)))</formula>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="58" priority="54" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E29">
-    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="55" priority="51" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="54" priority="52" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="50" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="53" priority="53" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28:N31 J28:K31">
-    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="52" priority="47" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="51" priority="48" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31">
-    <cfRule type="containsText" dxfId="42" priority="41" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="48" priority="44" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="43" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E25">
-    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="45" priority="41" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="44" priority="42" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="43" priority="43" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24:N27 J24:K27">
-    <cfRule type="containsText" dxfId="36" priority="34" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="42" priority="37" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="41" priority="38" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="37" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E27">
-    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E21">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20:N23 J20:K23">
-    <cfRule type="containsText" dxfId="26" priority="24" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="32" priority="27" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="31" priority="28" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="30" priority="29" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E23">
-    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="28" priority="24" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:E17">
-    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="25" priority="21" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16:N19 J16:K19">
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E13">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12:N15 J12:K15">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E15">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E10">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",E9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",E9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -3711,8 +3820,13 @@
     <hyperlink ref="I9" r:id="rId30"/>
     <hyperlink ref="O9" r:id="rId31"/>
     <hyperlink ref="P9" r:id="rId32"/>
+    <hyperlink ref="I10" r:id="rId33"/>
+    <hyperlink ref="Q9" r:id="rId34"/>
+    <hyperlink ref="R9" r:id="rId35"/>
+    <hyperlink ref="O10" r:id="rId36"/>
+    <hyperlink ref="P10" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape" r:id="rId33"/>
+  <pageSetup scale="60" orientation="landscape" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Find Duplicate in Array
</commit_message>
<xml_diff>
--- a/Resources/Index.xlsx
+++ b/Resources/Index.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="56">
   <si>
     <t>Sr No.</t>
   </si>
@@ -181,13 +181,22 @@
   </si>
   <si>
     <t>Even-Odd Calculation</t>
+  </si>
+  <si>
+    <t>Find Duplicate in Array</t>
+  </si>
+  <si>
+    <t>Hashing, Cycle Detection</t>
+  </si>
+  <si>
+    <t>Frequency Counting, Floyd's Tortoise and Hare (Cycle Detection)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,14 +234,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -555,25 +556,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -623,13 +615,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -662,16 +654,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1668,1768 +1657,1687 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="8" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="13" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="8" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="8.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31" t="s">
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="31" t="s">
+      <c r="P1" s="29"/>
+      <c r="Q1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="3"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="26" t="s">
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="34"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="26" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="3"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="31"/>
     </row>
-    <row r="3" spans="1:20" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="13" t="s">
+    <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="35"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="13" t="s">
+      <c r="L3" s="25"/>
+      <c r="M3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="8"/>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15">
+    <row r="4" spans="1:20" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" s="8"/>
-      <c r="T4" s="9" t="s">
+      <c r="I4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
+    <row r="5" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="S5" s="8"/>
-      <c r="T5" s="10" t="s">
+      <c r="I5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15">
+    <row r="6" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="S6" s="8"/>
-      <c r="T6" s="11" t="s">
+      <c r="I6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+    <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="R7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="S7" s="8"/>
-      <c r="T7" s="12" t="s">
+      <c r="I7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="1" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15">
+    <row r="8" spans="1:20" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="S8" s="8"/>
-      <c r="T8"/>
+      <c r="I8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="18" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="15">
+    <row r="9" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
         <v>6</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="19" t="s">
+      <c r="I9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="O9" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="S9" s="8"/>
-      <c r="T9" s="4" t="s">
+      <c r="O9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="15">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="19" t="s">
+      <c r="I10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="38" t="s">
+      <c r="M10" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="38" t="s">
+      <c r="N10" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="O10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="S10" s="8"/>
-      <c r="T10" s="4" t="s">
+      <c r="O10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15">
+    <row r="11" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="S11" s="8"/>
-      <c r="T11" s="5" t="s">
+      <c r="B11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15">
+      <c r="A12" s="12">
         <v>9</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="36" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="36" t="s">
+      <c r="L12" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="36" t="s">
+      <c r="N12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R12" s="20" t="s">
+      <c r="O12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R12" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="15">
+      <c r="A13" s="12">
         <v>10</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="37" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="37" t="s">
+      <c r="K13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="37" t="s">
+      <c r="L13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="37" t="s">
+      <c r="N13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" s="20" t="s">
+      <c r="O13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R13" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="15">
+      <c r="A14" s="12">
         <v>11</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="16" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="38" t="s">
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="38" t="s">
+      <c r="L14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N14" s="38" t="s">
+      <c r="N14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R14" s="20" t="s">
+      <c r="O14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R14" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="15">
+      <c r="A15" s="12">
         <v>12</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="16" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R15" s="20" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15">
+      <c r="A16" s="12">
         <v>13</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="36" t="s">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="36" t="s">
+      <c r="L16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="36" t="s">
+      <c r="N16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O16" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P16" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q16" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R16" s="20" t="s">
+      <c r="O16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R16" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
         <v>14</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="37" t="s">
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="37" t="s">
+      <c r="K17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="37" t="s">
+      <c r="L17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N17" s="37" t="s">
+      <c r="N17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P17" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q17" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R17" s="20" t="s">
+      <c r="O17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
         <v>15</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="16" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="38" t="s">
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K18" s="38" t="s">
+      <c r="K18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="38" t="s">
+      <c r="L18" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N18" s="38" t="s">
+      <c r="N18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R18" s="20" t="s">
+      <c r="O18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R18" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
         <v>16</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="16" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R19" s="20" t="s">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R19" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="15">
+    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12">
         <v>17</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="36" t="s">
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M20" s="36" t="s">
+      <c r="L20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="N20" s="36" t="s">
+      <c r="N20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O20" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P20" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q20" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R20" s="20" t="s">
+      <c r="O20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
         <v>18</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="37" t="s">
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K21" s="37" t="s">
+      <c r="K21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L21" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="37" t="s">
+      <c r="L21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N21" s="37" t="s">
+      <c r="N21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O21" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P21" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q21" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R21" s="20" t="s">
+      <c r="O21" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P21" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q21" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R21" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="12">
         <v>19</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="16" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="38" t="s">
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="38" t="s">
+      <c r="K22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M22" s="38" t="s">
+      <c r="L22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="38" t="s">
+      <c r="N22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O22" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P22" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q22" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R22" s="20" t="s">
+      <c r="O22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="15">
-        <v>20</v>
-      </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="16" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>20</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O23" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P23" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q23" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R23" s="20" t="s">
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R23" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="15">
-        <v>21</v>
-      </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16" t="s">
+    <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12">
+        <v>21</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="36" t="s">
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K24" s="36" t="s">
+      <c r="K24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M24" s="36" t="s">
+      <c r="L24" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="N24" s="36" t="s">
+      <c r="N24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O24" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P24" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q24" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R24" s="20" t="s">
+      <c r="O24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R24" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="12">
         <v>22</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="37" t="s">
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K25" s="37" t="s">
+      <c r="K25" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="37" t="s">
+      <c r="L25" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N25" s="37" t="s">
+      <c r="N25" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O25" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P25" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q25" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R25" s="20" t="s">
+      <c r="O25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R25" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
         <v>23</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="16" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="38" t="s">
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="38" t="s">
+      <c r="K26" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L26" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M26" s="38" t="s">
+      <c r="L26" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N26" s="38" t="s">
+      <c r="N26" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O26" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P26" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q26" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R26" s="20" t="s">
+      <c r="O26" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q26" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R26" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="12">
         <v>24</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="16" t="s">
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M27" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N27" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O27" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P27" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R27" s="20" t="s">
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O27" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P27" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R27" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="15">
+    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12">
         <v>25</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J28" s="36" t="s">
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K28" s="36" t="s">
+      <c r="K28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L28" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M28" s="36" t="s">
+      <c r="L28" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="N28" s="36" t="s">
+      <c r="N28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O28" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P28" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R28" s="20" t="s">
+      <c r="O28" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R28" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
         <v>26</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="37" t="s">
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="37" t="s">
+      <c r="K29" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L29" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M29" s="37" t="s">
+      <c r="L29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N29" s="37" t="s">
+      <c r="N29" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O29" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P29" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R29" s="20" t="s">
+      <c r="O29" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P29" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q29" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R29" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="12">
         <v>27</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="16" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="38" t="s">
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K30" s="38" t="s">
+      <c r="K30" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L30" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M30" s="38" t="s">
+      <c r="L30" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N30" s="38" t="s">
+      <c r="N30" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O30" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P30" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R30" s="20" t="s">
+      <c r="O30" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P30" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q30" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R30" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="12">
         <v>28</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="16" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M31" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O31" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P31" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q31" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R31" s="20" t="s">
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R31" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="15">
+    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="12">
         <v>29</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16" t="s">
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="36" t="s">
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K32" s="36" t="s">
+      <c r="K32" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L32" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M32" s="36" t="s">
+      <c r="L32" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M32" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="N32" s="36" t="s">
+      <c r="N32" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O32" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P32" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q32" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R32" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="T32" s="3"/>
+      <c r="O32" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P32" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q32" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R32" s="17" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="15">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="12">
         <v>30</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17" t="s">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="37" t="s">
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K33" s="37" t="s">
+      <c r="K33" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L33" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M33" s="37" t="s">
+      <c r="L33" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N33" s="37" t="s">
+      <c r="N33" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O33" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P33" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q33" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R33" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="T33" s="3"/>
+      <c r="O33" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P33" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R33" s="17" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" s="15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="12">
         <v>31</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="16" t="s">
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="38" t="s">
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K34" s="38" t="s">
+      <c r="K34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L34" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" s="38" t="s">
+      <c r="L34" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N34" s="38" t="s">
+      <c r="N34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O34" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P34" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q34" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R34" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="T34" s="3"/>
+      <c r="O34" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P34" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q34" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R34" s="17" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" s="15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="12">
         <v>32</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="16" t="s">
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L35" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="N35" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O35" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="P35" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q35" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R35" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="T35" s="3"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O35" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P35" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q35" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R35" s="17" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="T36" s="3"/>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" s="39"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="E39"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="E40"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B41"/>
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B42"/>
-      <c r="D42"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:T3"/>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="I1:N1"/>
@@ -3440,351 +3348,346 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J7">
-    <cfRule type="containsText" dxfId="97" priority="95" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="96" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="97" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="95" priority="100" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="94" priority="101" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K7">
-    <cfRule type="containsText" dxfId="93" priority="91" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="93" priority="94" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="92" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="92" priority="95" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="93" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="91" priority="96" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="90" priority="97" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N7">
-    <cfRule type="containsText" dxfId="89" priority="87" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="89" priority="90" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="88" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="88" priority="91" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="89" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="87" priority="92" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="90" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="86" priority="93" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",M4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:T7">
-    <cfRule type="containsText" dxfId="85" priority="83" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="84" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="85" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="83" priority="88" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="82" priority="89" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",T4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 E6:E7 E32:E33">
-    <cfRule type="containsText" dxfId="81" priority="80" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="81" priority="83" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="80" priority="84" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="82" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="79" priority="85" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T9:T11">
-    <cfRule type="containsText" dxfId="78" priority="77" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="78" priority="80" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",T9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="77" priority="81" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",T9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="79" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="76" priority="82" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",T9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32:N35 J32:K35">
-    <cfRule type="containsText" dxfId="75" priority="73" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="74" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="74" priority="77" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="75" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="73" priority="78" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="76" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="72" priority="79" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E35">
-    <cfRule type="containsText" dxfId="71" priority="67" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="68" priority="64" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="65" priority="61" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="62" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:N11 J8:K11">
-    <cfRule type="containsText" dxfId="62" priority="57" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="62" priority="60" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="58" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="61" priority="61" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="59" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="60" priority="62" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="59" priority="63" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:E29">
+    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M28:N31 J28:K31">
+    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",J28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",J28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="Attempted">
+      <formula>NOT(ISERROR(SEARCH("Attempted",J28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",J28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30:E31">
+    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="49" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:E25">
+    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="46" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M24:N27 J24:K27">
+    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",J24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",J24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="Attempted">
+      <formula>NOT(ISERROR(SEARCH("Attempted",J24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",J24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:E27">
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E21">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M20:N23 J20:K23">
+    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",J20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",J20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="Attempted">
+      <formula>NOT(ISERROR(SEARCH("Attempted",J20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",J20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E23">
+    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E17">
+    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M16:N19 J16:K19">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",J16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",J16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Attempted">
+      <formula>NOT(ISERROR(SEARCH("Attempted",J16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",J16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E19">
+    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E13">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12:N15 J12:K15">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Attempted">
+      <formula>NOT(ISERROR(SEARCH("Attempted",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E15">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E10">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="58" priority="54" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E29">
-    <cfRule type="containsText" dxfId="55" priority="51" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="52" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="53" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M28:N31 J28:K31">
-    <cfRule type="containsText" dxfId="52" priority="47" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="48" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E31">
-    <cfRule type="containsText" dxfId="48" priority="44" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24:E25">
-    <cfRule type="containsText" dxfId="45" priority="41" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="42" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="43" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M24:N27 J24:K27">
-    <cfRule type="containsText" dxfId="42" priority="37" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="38" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E27">
-    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E21">
-    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M20:N23 J20:K23">
-    <cfRule type="containsText" dxfId="32" priority="27" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="28" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="29" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E23">
-    <cfRule type="containsText" dxfId="28" priority="24" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16:E17">
-    <cfRule type="containsText" dxfId="25" priority="21" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M16:N19 J16:K19">
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E19">
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E13">
-    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M12:N15 J12:K15">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E15">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:E10">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -3825,8 +3728,14 @@
     <hyperlink ref="R9" r:id="rId35"/>
     <hyperlink ref="O10" r:id="rId36"/>
     <hyperlink ref="P10" r:id="rId37"/>
+    <hyperlink ref="Q10" r:id="rId38"/>
+    <hyperlink ref="R10" r:id="rId39"/>
+    <hyperlink ref="I11" r:id="rId40"/>
+    <hyperlink ref="L11" r:id="rId41"/>
+    <hyperlink ref="O11" r:id="rId42"/>
+    <hyperlink ref="P11" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape" r:id="rId38"/>
+  <pageSetup scale="60" orientation="landscape" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Find All Duplicates in Array
</commit_message>
<xml_diff>
--- a/Resources/Index.xlsx
+++ b/Resources/Index.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="59">
   <si>
     <t>Sr No.</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>Frequency Counting, Floyd's Tortoise and Hare (Cycle Detection)</t>
+  </si>
+  <si>
+    <t>Find All Duplicates in Array</t>
+  </si>
+  <si>
+    <t>Two Pointers, Frequency Counting</t>
+  </si>
+  <si>
+    <t>Commonly Asked</t>
   </si>
 </sst>
 </file>
@@ -624,6 +633,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -652,15 +670,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -735,6 +744,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1037,27 +1067,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1660,8 +1669,8 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1690,93 +1699,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="28" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="28" t="s">
+      <c r="P1" s="32"/>
+      <c r="Q1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="29"/>
+      <c r="R1" s="32"/>
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="23" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="23" t="s">
+      <c r="K2" s="30"/>
+      <c r="L2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="31"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="34"/>
     </row>
     <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="25"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="10" t="s">
         <v>12</v>
       </c>
@@ -2255,51 +2264,63 @@
       <c r="P11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11" s="17" t="s">
+      <c r="Q11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11" s="18" t="s">
         <v>20</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>9</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="E12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="16" t="s">
+      <c r="H12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>20</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="18" t="s">
         <v>20</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="18" t="s">
         <v>20</v>
       </c>
       <c r="Q12" s="17" t="s">
@@ -2750,594 +2771,56 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="12">
-        <v>20</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="O23" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P23" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q23" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R23" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12">
-        <v>21</v>
-      </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="N24" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="O24" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P24" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q24" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R24" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="12">
-        <v>22</v>
-      </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K25" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="N25" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="O25" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P25" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q25" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R25" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A25" s="5"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="12">
-        <v>23</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="K26" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="L26" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M26" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="N26" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="O26" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P26" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q26" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R26" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A26" s="5"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="12">
-        <v>24</v>
-      </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N27" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="O27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R27" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12">
-        <v>25</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="K28" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M28" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="N28" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="O28" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P28" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R28" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A27" s="5"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="12">
-        <v>26</v>
-      </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K29" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M29" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="N29" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="O29" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P29" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R29" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A29" s="5"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="12">
-        <v>27</v>
-      </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="K30" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="L30" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M30" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="N30" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="O30" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P30" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R30" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A30" s="5"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="12">
-        <v>28</v>
-      </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M31" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="O31" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P31" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q31" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R31" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="12">
-        <v>29</v>
-      </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M32" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="N32" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="O32" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P32" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q32" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R32" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="12">
-        <v>30</v>
-      </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K33" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M33" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="N33" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="O33" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P33" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q33" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R33" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="12">
-        <v>31</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="K34" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="N34" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="O34" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P34" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q34" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R34" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="12">
-        <v>32</v>
-      </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N35" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="O35" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P35" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q35" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R35" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:T3"/>
   <mergeCells count="15">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="I1:N1"/>
@@ -3348,346 +2831,265 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="H1:H3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J7">
-    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="96" priority="102" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="100" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="95" priority="103" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="101" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="94" priority="104" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K7">
-    <cfRule type="containsText" dxfId="93" priority="94" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="93" priority="97" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="95" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="92" priority="98" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="96" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="91" priority="99" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="97" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="90" priority="100" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N7">
-    <cfRule type="containsText" dxfId="89" priority="90" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="89" priority="93" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="91" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="88" priority="94" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="92" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="87" priority="95" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="93" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="86" priority="96" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",M4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:T7">
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="84" priority="90" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="88" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="83" priority="91" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="89" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="82" priority="92" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",T4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 E6:E7 E32:E33">
-    <cfRule type="containsText" dxfId="81" priority="83" operator="containsText" text="Hard">
+  <conditionalFormatting sqref="E4 E6:E7">
+    <cfRule type="containsText" dxfId="81" priority="86" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="84" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="80" priority="87" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="85" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="79" priority="88" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T9:T11">
-    <cfRule type="containsText" dxfId="78" priority="80" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="78" priority="83" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",T9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="81" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="77" priority="84" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",T9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="82" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="76" priority="85" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",T9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M32:N35 J32:K35">
-    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="77" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="78" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="79" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34:E35">
-    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:N11 J8:K11">
-    <cfRule type="containsText" dxfId="62" priority="60" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="61" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="61" priority="64" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="62" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="60" priority="65" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="63" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="59" priority="66" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E29">
-    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M28:N31 J28:K31">
-    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E31">
-    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="49" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24:E25">
-    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="46" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M24:N27 J24:K27">
-    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E27">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E21">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20:N23 J20:K23">
-    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="Done">
+  <conditionalFormatting sqref="M20:N22 J20:K22">
+    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E23">
-    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="Hard">
+  <conditionalFormatting sqref="E22">
+    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:E17">
-    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16:N19 J16:K19">
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
+    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
     <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",E13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",E13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E13">
-    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12:N15 J12:K15">
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E15">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E10">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Hard",E12)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Medium",E12)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Easy",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -3734,8 +3136,14 @@
     <hyperlink ref="L11" r:id="rId41"/>
     <hyperlink ref="O11" r:id="rId42"/>
     <hyperlink ref="P11" r:id="rId43"/>
+    <hyperlink ref="Q11" r:id="rId44"/>
+    <hyperlink ref="R11" r:id="rId45"/>
+    <hyperlink ref="I12" r:id="rId46"/>
+    <hyperlink ref="L12" r:id="rId47"/>
+    <hyperlink ref="O12" r:id="rId48"/>
+    <hyperlink ref="P12" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape" r:id="rId44"/>
+  <pageSetup scale="60" orientation="landscape" r:id="rId50"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Unique no of Occurrences
</commit_message>
<xml_diff>
--- a/Resources/Index.xlsx
+++ b/Resources/Index.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="62">
   <si>
     <t>Sr No.</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>Commonly Asked</t>
+  </si>
+  <si>
+    <t>Unique no of Occurrences</t>
+  </si>
+  <si>
+    <t>Frequency Count</t>
+  </si>
+  <si>
+    <t>Hash Map, Frequency Count</t>
   </si>
 </sst>
 </file>
@@ -677,7 +686,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="74">
     <dxf>
       <fill>
         <patternFill>
@@ -765,6 +774,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -954,6 +984,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -975,34 +1033,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1018,195 +1048,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1669,8 +1510,8 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2323,48 +2164,60 @@
       <c r="P12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R12" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R12" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>10</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="B13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="I13" s="16" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="18" t="s">
         <v>20</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" s="18" t="s">
         <v>20</v>
       </c>
       <c r="Q13" s="17" t="s">
@@ -2838,258 +2691,258 @@
     <mergeCell ref="E1:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J7">
-    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="73" priority="104" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="102" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="72" priority="105" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="103" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="71" priority="106" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="104" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="70" priority="107" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K7">
-    <cfRule type="containsText" dxfId="93" priority="97" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="69" priority="100" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="98" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="68" priority="101" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="99" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="67" priority="102" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="100" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="66" priority="103" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N7">
-    <cfRule type="containsText" dxfId="89" priority="93" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="65" priority="96" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="94" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="64" priority="97" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="95" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="63" priority="98" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",M4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="96" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="62" priority="99" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",M4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:T7">
-    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="61" priority="92" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="90" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="60" priority="93" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="91" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="59" priority="94" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="92" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="58" priority="95" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",T4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 E6:E7">
-    <cfRule type="containsText" dxfId="81" priority="86" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="57" priority="89" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="87" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="56" priority="90" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="88" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="55" priority="91" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T9:T11">
-    <cfRule type="containsText" dxfId="78" priority="83" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="54" priority="86" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",T9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="84" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="53" priority="87" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",T9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="85" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="52" priority="88" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",T9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="51" priority="73" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="50" priority="74" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="49" priority="75" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="48" priority="70" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="47" priority="71" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="46" priority="72" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:N11 J8:K11">
-    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="45" priority="66" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="64" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="44" priority="67" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="65" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="43" priority="68" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="66" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="42" priority="69" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E21">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20:N22 J20:K22">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="38" priority="36" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="37" priority="37" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="36" priority="38" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="34" priority="33" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="32" priority="35" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:E17">
-    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16:N19 J16:K19">
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Attempted">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Attempted">
       <formula>NOT(ISERROR(SEARCH("Attempted",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
-    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12:N15 J12:K15">
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Attempted">
+      <formula>NOT(ISERROR(SEARCH("Attempted",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E15">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E10">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",E13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M12:N15 J12:K15">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Attempted">
-      <formula>NOT(ISERROR(SEARCH("Attempted",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",J12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E15">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:E10">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
-      <formula>NOT(ISERROR(SEARCH("Hard",E12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",E12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",E12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -3142,8 +2995,13 @@
     <hyperlink ref="L12" r:id="rId47"/>
     <hyperlink ref="O12" r:id="rId48"/>
     <hyperlink ref="P12" r:id="rId49"/>
+    <hyperlink ref="Q12" r:id="rId50"/>
+    <hyperlink ref="R12" r:id="rId51"/>
+    <hyperlink ref="L13" r:id="rId52"/>
+    <hyperlink ref="O13" r:id="rId53"/>
+    <hyperlink ref="P13" r:id="rId54"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape" r:id="rId50"/>
+  <pageSetup scale="60" orientation="landscape" r:id="rId55"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Best Time to Buy and Sell Stock II – Multiple Transaction Allowed
</commit_message>
<xml_diff>
--- a/Resources/Index.xlsx
+++ b/Resources/Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Muzammil\Coding\04-DSA\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AD18E0-BE98-48DD-9542-98FFB84C0DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E0B147-0C5E-4CD1-A3BC-08E4F77D7863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="99">
   <si>
     <t>Sr No.</t>
   </si>
@@ -301,7 +301,25 @@
     <t>Custom Thresholds, Optimization</t>
   </si>
   <si>
-    <t>Best Time to Buy and Sell Stock I -  Max one Transaction Allowed</t>
+    <t>Best Time to Buy and Sell Stock I - Max one Transaction Allowed</t>
+  </si>
+  <si>
+    <t>Kadane’s Algorithm</t>
+  </si>
+  <si>
+    <t>Maximum Profit Problem</t>
+  </si>
+  <si>
+    <t>Greedy, Sliding Window</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock II – Multiple Transaction Allowed</t>
+  </si>
+  <si>
+    <t>Greedy Algorithm</t>
+  </si>
+  <si>
+    <t>Greedy, Stock Trading</t>
   </si>
 </sst>
 </file>
@@ -729,6 +747,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -744,15 +783,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -760,18 +790,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1245,9 +1263,9 @@
   </sheetPr>
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,110 +1294,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="36" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="37"/>
-      <c r="T1" s="36" t="s">
+      <c r="S1" s="26"/>
+      <c r="T1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="37"/>
+      <c r="U1" s="26"/>
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="31"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="25" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="25" t="s">
+      <c r="K2" s="36"/>
+      <c r="L2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="29"/>
-      <c r="O2" s="25" t="s">
+      <c r="N2" s="36"/>
+      <c r="O2" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="P2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="39"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="28"/>
     </row>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="32"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
       <c r="J3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="27"/>
+      <c r="L3" s="34"/>
       <c r="M3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="27"/>
+      <c r="O3" s="34"/>
       <c r="P3" s="10" t="s">
         <v>12</v>
       </c>
@@ -2600,13 +2618,21 @@
       <c r="C22" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="24"/>
+      <c r="D22" s="24" t="s">
+        <v>93</v>
+      </c>
       <c r="E22" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="I22" s="18" t="s">
         <v>20</v>
       </c>
@@ -2640,25 +2666,39 @@
       <c r="S22" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="T22" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="U22" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T22" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="U22" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>20</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="16" t="s">
+      <c r="B23" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" s="18" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="22" t="s">
@@ -2667,7 +2707,7 @@
       <c r="K23" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="L23" s="16" t="s">
+      <c r="L23" s="18" t="s">
         <v>20</v>
       </c>
       <c r="M23" s="22" t="s">
@@ -2676,7 +2716,7 @@
       <c r="N23" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="16" t="s">
+      <c r="O23" s="18" t="s">
         <v>20</v>
       </c>
       <c r="P23" s="22" t="s">
@@ -2685,10 +2725,10 @@
       <c r="Q23" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="S23" s="17" t="s">
+      <c r="R23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="S23" s="18" t="s">
         <v>20</v>
       </c>
       <c r="T23" s="17" t="s">
@@ -3960,6 +4000,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R1:S2"/>
     <mergeCell ref="T1:U2"/>
     <mergeCell ref="A1:A3"/>
@@ -3976,7 +4017,6 @@
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:Q1"/>
     <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E47">
     <cfRule type="containsText" dxfId="22" priority="69" operator="containsText" text="Hard">
@@ -4170,13 +4210,19 @@
     <hyperlink ref="S21" r:id="rId106" xr:uid="{2F09247B-2764-4ACB-BEFD-7A503F06D8BE}"/>
     <hyperlink ref="T21" r:id="rId107" xr:uid="{6175F423-FCEB-45D6-A7A5-765AA65D6B0F}"/>
     <hyperlink ref="U21" r:id="rId108" xr:uid="{8EBF5379-AA47-418A-A685-7D9501E41ABC}"/>
-    <hyperlink ref="B22" r:id="rId109" display="https://leetcode.com/problems/best-time-to-buy-and-sell-stock/" xr:uid="{3981297C-69B8-4F6D-B97B-DA2B315F8298}"/>
-    <hyperlink ref="I22" r:id="rId110" xr:uid="{19354754-5793-45A1-BB19-0616F3B189FB}"/>
-    <hyperlink ref="O22" r:id="rId111" xr:uid="{DF4C506B-0778-4E9F-9805-AC1A5A851200}"/>
-    <hyperlink ref="R22" r:id="rId112" xr:uid="{7AA405A6-169D-4F3A-BF66-6C7F902C9D29}"/>
-    <hyperlink ref="S22" r:id="rId113" xr:uid="{5C3DD2D9-686B-4D86-BC03-B058EB724F99}"/>
+    <hyperlink ref="I22" r:id="rId109" xr:uid="{19354754-5793-45A1-BB19-0616F3B189FB}"/>
+    <hyperlink ref="O22" r:id="rId110" xr:uid="{DF4C506B-0778-4E9F-9805-AC1A5A851200}"/>
+    <hyperlink ref="R22" r:id="rId111" xr:uid="{7AA405A6-169D-4F3A-BF66-6C7F902C9D29}"/>
+    <hyperlink ref="S22" r:id="rId112" xr:uid="{5C3DD2D9-686B-4D86-BC03-B058EB724F99}"/>
+    <hyperlink ref="T22" r:id="rId113" xr:uid="{2B4F71E6-7EF8-4EFD-B476-81DF28E6B3D0}"/>
+    <hyperlink ref="U22" r:id="rId114" xr:uid="{6856A36B-E306-4F72-A98B-C4D962667BAB}"/>
+    <hyperlink ref="L23" r:id="rId115" xr:uid="{351D3751-C6CB-451D-A01B-FBC9892045C6}"/>
+    <hyperlink ref="O23" r:id="rId116" xr:uid="{ECB05E46-5E71-416B-A33B-C660C4776BBB}"/>
+    <hyperlink ref="I23" r:id="rId117" xr:uid="{6D30BFF8-2566-4A23-A316-F0191A8CDBC1}"/>
+    <hyperlink ref="R23" r:id="rId118" xr:uid="{F44D82E5-B56F-4D5A-8BB8-F8A58AB3FC9B}"/>
+    <hyperlink ref="S23" r:id="rId119" xr:uid="{5E1923B8-141F-4486-8A4D-0057FAE79671}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape" r:id="rId114"/>
+  <pageSetup scale="60" orientation="landscape" r:id="rId120"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minimize the Heights II
</commit_message>
<xml_diff>
--- a/Resources/Index.xlsx
+++ b/Resources/Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Muzammil\Coding\04-DSA\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E0B147-0C5E-4CD1-A3BC-08E4F77D7863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DCA56B-EC48-4135-9BD5-80E2754EA199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="103">
   <si>
     <t>Sr No.</t>
   </si>
@@ -320,6 +320,18 @@
   </si>
   <si>
     <t>Greedy, Stock Trading</t>
+  </si>
+  <si>
+    <t>Minimize the Heights II</t>
+  </si>
+  <si>
+    <t>Sorting, Greedy</t>
+  </si>
+  <si>
+    <t>Min-Max Problem</t>
+  </si>
+  <si>
+    <t>Optimization, Range Adjustment</t>
   </si>
 </sst>
 </file>
@@ -1263,9 +1275,9 @@
   </sheetPr>
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2731,57 +2743,69 @@
       <c r="S23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="T23" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="U23" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="U23" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>21</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
+      <c r="B24" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>100</v>
+      </c>
       <c r="E24" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="F24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>102</v>
+      </c>
       <c r="I24" s="16" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="N24" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="O24" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24" s="18" t="s">
         <v>20</v>
       </c>
       <c r="P24" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q24" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="R24" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="S24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="S24" s="18" t="s">
         <v>20</v>
       </c>
       <c r="T24" s="17" t="s">
@@ -4221,8 +4245,13 @@
     <hyperlink ref="I23" r:id="rId117" xr:uid="{6D30BFF8-2566-4A23-A316-F0191A8CDBC1}"/>
     <hyperlink ref="R23" r:id="rId118" xr:uid="{F44D82E5-B56F-4D5A-8BB8-F8A58AB3FC9B}"/>
     <hyperlink ref="S23" r:id="rId119" xr:uid="{5E1923B8-141F-4486-8A4D-0057FAE79671}"/>
+    <hyperlink ref="T23" r:id="rId120" xr:uid="{7E35E8A2-785F-45D0-91BA-1FB8573C263F}"/>
+    <hyperlink ref="U23" r:id="rId121" xr:uid="{E24B265F-0433-4BBE-8FD0-849562C71D39}"/>
+    <hyperlink ref="O24" r:id="rId122" xr:uid="{02EAB5B4-2537-4941-AA18-A064194FEAED}"/>
+    <hyperlink ref="R24" r:id="rId123" xr:uid="{693A97D6-8E44-430E-8B91-875763F3F6AD}"/>
+    <hyperlink ref="S24" r:id="rId124" xr:uid="{CCB32ED6-B113-4B87-8362-0DCAFF7417E2}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape" r:id="rId120"/>
+  <pageSetup scale="60" orientation="landscape" r:id="rId125"/>
 </worksheet>
 </file>
</xml_diff>